<commit_message>
Pre-Lone Star code, pre-clean up
</commit_message>
<xml_diff>
--- a/DistanceCalc.xlsx
+++ b/DistanceCalc.xlsx
@@ -16,30 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Key length</t>
+    <t>Target Height (from center of mass to image bottom)</t>
   </si>
   <si>
-    <t>Fender</t>
-  </si>
-  <si>
-    <t>Top basket</t>
-  </si>
-  <si>
-    <t>Inches</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Img Ht</t>
-  </si>
-  <si>
-    <t>For 90" tall basket</t>
-  </si>
-  <si>
-    <t>Keep in mind that top left of image is (0,0)</t>
+    <t>Real Life distance</t>
   </si>
 </sst>
 </file>
@@ -75,9 +57,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -85,132 +66,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$3:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>72</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$3:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>127</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>188</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="68233472"/>
-        <c:axId val="68231936"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="68233472"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68231936"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="68231936"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68233472"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,83 +353,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <f>240-80</f>
+        <v>160</v>
       </c>
       <c r="B2">
-        <v>144</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
+        <v>96.75</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>38.75</v>
-      </c>
-      <c r="D3">
-        <v>160</v>
-      </c>
-      <c r="E3">
-        <v>83</v>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <f>240-85</f>
+        <v>155</v>
+      </c>
+      <c r="B3">
+        <v>104.625</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <f>240-108</f>
+        <v>132</v>
       </c>
       <c r="B4">
-        <v>98</v>
-      </c>
-      <c r="D4">
-        <v>102</v>
-      </c>
-      <c r="E4">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="D5">
-        <v>72</v>
-      </c>
-      <c r="E5">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>7</v>
+        <v>126.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>